<commit_message>
Agregado Alta PP MainFrame
</commit_message>
<xml_diff>
--- a/MyFirstTest/registers.xlsx
+++ b/MyFirstTest/registers.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seolivera\Documents\GitHub\Automatizaci-nTFNU\MyFirstTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seba-OS\Documents\GitHub\Automatizaci-nTFNU\MyFirstTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752C8C45-F59A-48E6-BF98-3798EB882154}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14796" windowHeight="7656"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="POTENTIAL-RESCLIENTS" sheetId="1" r:id="rId1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="50">
   <si>
     <t>UAT</t>
   </si>
@@ -153,31 +154,37 @@
     <t>https://noprd-uat-toms.temu.com.uy:7002/common/uobject.jsp?object=9157332706713843846</t>
   </si>
   <si>
-    <t>89598071103029413716</t>
-  </si>
-  <si>
-    <t>93655923</t>
-  </si>
-  <si>
-    <t>PLR3</t>
-  </si>
-  <si>
-    <t>Puper</t>
-  </si>
-  <si>
-    <t>Puper2</t>
-  </si>
-  <si>
-    <t>8877660038</t>
-  </si>
-  <si>
-    <t>8877660037</t>
+    <t>PLR310</t>
+  </si>
+  <si>
+    <t>93821778</t>
+  </si>
+  <si>
+    <t>89598071103029413799</t>
+  </si>
+  <si>
+    <t>NativoAutomation1</t>
+  </si>
+  <si>
+    <t>NativoAutomation2</t>
+  </si>
+  <si>
+    <t>Prueba</t>
+  </si>
+  <si>
+    <t>Prueba2</t>
+  </si>
+  <si>
+    <t>8877660031</t>
+  </si>
+  <si>
+    <t>8877660032</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="21">
     <font>
       <sz val="11"/>
@@ -1039,11 +1046,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1077,13 +1084,13 @@
         <v>21</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>7</v>
@@ -1094,13 +1101,13 @@
         <v>21</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>7</v>
@@ -1113,7 +1120,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1155,7 +1162,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1219,7 +1226,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1276,7 +1283,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1332,11 +1339,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1373,10 +1380,10 @@
         <v>36</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>42</v>
@@ -1389,7 +1396,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1427,7 +1434,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -1435,7 +1442,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1487,7 +1494,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1520,7 +1527,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://noprd-e2e-toms.temu.com.uy:7002/common/uobject.jsp?object=9157101132513589622"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://noprd-e2e-toms.temu.com.uy:7002/common/uobject.jsp?object=9157101132513589622" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -1528,7 +1535,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Add option passport or international id
Se adiciona condicion a la hora de crear Clientes,con pasaporte o cedula
</commit_message>
<xml_diff>
--- a/MyFirstTest/registers.xlsx
+++ b/MyFirstTest/registers.xlsx
@@ -1,35 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20344"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ipupo\Documents\GitHub\Automatizaci-nTFNU\MyFirstTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5F1202-8A2A-4D4F-93DC-AB2773CF19C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{8CB5995E-E8E4-4ADD-869D-6A6EA7EBB9ED}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14790" windowHeight="7650" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="3" windowHeight="7650" windowWidth="14790" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="POTENTIAL-RESCLIENTS" sheetId="1" r:id="rId1"/>
-    <sheet name="POTENTIAL-ENTCLIENTS" sheetId="3" r:id="rId2"/>
-    <sheet name="REAL-RESCLIENTS" sheetId="2" r:id="rId3"/>
-    <sheet name="REAL-ENTCLIENTS" sheetId="4" r:id="rId4"/>
-    <sheet name="NEW-PLAN" sheetId="5" r:id="rId5"/>
-    <sheet name="REAL-PLAN" sheetId="6" r:id="rId6"/>
-    <sheet name="CHANGE-PLAN" sheetId="7" r:id="rId7"/>
-    <sheet name="CHANGED-PLAN" sheetId="8" r:id="rId8"/>
-    <sheet name="SIM CARD LOST" sheetId="9" r:id="rId9"/>
-    <sheet name="REGISTERED SIM CARD LOST" sheetId="10" r:id="rId10"/>
+    <sheet name="POTENTIAL-RESCLIENTS" r:id="rId1" sheetId="1"/>
+    <sheet name="POTENTIAL-ENTCLIENTS" r:id="rId2" sheetId="3"/>
+    <sheet name="REAL-RESCLIENTS" r:id="rId3" sheetId="2"/>
+    <sheet name="REAL-ENTCLIENTS" r:id="rId4" sheetId="4"/>
+    <sheet name="NEW-PLAN" r:id="rId5" sheetId="5"/>
+    <sheet name="REAL-PLAN" r:id="rId6" sheetId="6"/>
+    <sheet name="CHANGE-PLAN" r:id="rId7" sheetId="7"/>
+    <sheet name="CHANGED-PLAN" r:id="rId8" sheetId="8"/>
+    <sheet name="SIM CARD LOST" r:id="rId9" sheetId="9"/>
+    <sheet name="REGISTERED SIM CARD LOST" r:id="rId10" sheetId="10"/>
+    <sheet name="RECHARGE LINE" r:id="rId11" sheetId="11"/>
+    <sheet name="REGISTERED RECHARGE" r:id="rId12" sheetId="12"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="49">
   <si>
     <t>UAT</t>
   </si>
@@ -43,9 +45,6 @@
     <t>SECOND NAME</t>
   </si>
   <si>
-    <t>DNI</t>
-  </si>
-  <si>
     <t>ADDRESS</t>
   </si>
   <si>
@@ -103,9 +102,6 @@
     <t>NativoAuto2Emp</t>
   </si>
   <si>
-    <t>11558877112</t>
-  </si>
-  <si>
     <t>210712640045</t>
   </si>
   <si>
@@ -124,15 +120,9 @@
     <t>Pupo</t>
   </si>
   <si>
-    <t>009988112233</t>
-  </si>
-  <si>
     <t>https://noprd-uat-toms.temu.com.uy:7002/common/uobject.jsp?object=9157298777113287522</t>
   </si>
   <si>
-    <t>89598076103021044159</t>
-  </si>
-  <si>
     <t>NativoAutomation5</t>
   </si>
   <si>
@@ -161,12 +151,40 @@
   </si>
   <si>
     <t>PLR3</t>
+  </si>
+  <si>
+    <t>LINE</t>
+  </si>
+  <si>
+    <t>LINK RECHARGE</t>
+  </si>
+  <si>
+    <t>TOTAL RECHARGE</t>
+  </si>
+  <si>
+    <t>PASSPORT</t>
+  </si>
+  <si>
+    <t>NATIONAL ID</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>9155890523813779409&amp;tab=_All+Tasks</t>
+  </si>
+  <si>
+    <t>22222222</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="21">
     <font>
       <sz val="11"/>
@@ -620,107 +638,107 @@
     </border>
   </borders>
   <cellStyleXfs count="43">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="0" fontId="4" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="5" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="2" fontId="6" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="7" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="5" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="6" fontId="10" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="6" fontId="11" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="6" fillId="0" fontId="12" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="7" fontId="13" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="14" numFmtId="0"/>
+    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="8" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="15" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="0" fontId="16" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="17" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="17" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="17" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="19" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="17" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="25" fontId="17" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="26" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="27" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="17" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="30" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="20" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="16" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="19" numFmtId="49" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="18" numFmtId="49" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="42"/>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Hipervínculo" xfId="42" builtinId="8"/>
-    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle builtinId="30" customBuiltin="1" name="20% - Énfasis1" xfId="19"/>
+    <cellStyle builtinId="34" customBuiltin="1" name="20% - Énfasis2" xfId="23"/>
+    <cellStyle builtinId="38" customBuiltin="1" name="20% - Énfasis3" xfId="27"/>
+    <cellStyle builtinId="42" customBuiltin="1" name="20% - Énfasis4" xfId="31"/>
+    <cellStyle builtinId="46" customBuiltin="1" name="20% - Énfasis5" xfId="35"/>
+    <cellStyle builtinId="50" customBuiltin="1" name="20% - Énfasis6" xfId="39"/>
+    <cellStyle builtinId="31" customBuiltin="1" name="40% - Énfasis1" xfId="20"/>
+    <cellStyle builtinId="35" customBuiltin="1" name="40% - Énfasis2" xfId="24"/>
+    <cellStyle builtinId="39" customBuiltin="1" name="40% - Énfasis3" xfId="28"/>
+    <cellStyle builtinId="43" customBuiltin="1" name="40% - Énfasis4" xfId="32"/>
+    <cellStyle builtinId="47" customBuiltin="1" name="40% - Énfasis5" xfId="36"/>
+    <cellStyle builtinId="51" customBuiltin="1" name="40% - Énfasis6" xfId="40"/>
+    <cellStyle builtinId="32" customBuiltin="1" name="60% - Énfasis1" xfId="21"/>
+    <cellStyle builtinId="36" customBuiltin="1" name="60% - Énfasis2" xfId="25"/>
+    <cellStyle builtinId="40" customBuiltin="1" name="60% - Énfasis3" xfId="29"/>
+    <cellStyle builtinId="44" customBuiltin="1" name="60% - Énfasis4" xfId="33"/>
+    <cellStyle builtinId="48" customBuiltin="1" name="60% - Énfasis5" xfId="37"/>
+    <cellStyle builtinId="52" customBuiltin="1" name="60% - Énfasis6" xfId="41"/>
+    <cellStyle builtinId="26" customBuiltin="1" name="Bueno" xfId="6"/>
+    <cellStyle builtinId="22" customBuiltin="1" name="Cálculo" xfId="11"/>
+    <cellStyle builtinId="23" customBuiltin="1" name="Celda de comprobación" xfId="13"/>
+    <cellStyle builtinId="24" customBuiltin="1" name="Celda vinculada" xfId="12"/>
+    <cellStyle builtinId="16" customBuiltin="1" name="Encabezado 1" xfId="2"/>
+    <cellStyle builtinId="19" customBuiltin="1" name="Encabezado 4" xfId="5"/>
+    <cellStyle builtinId="29" customBuiltin="1" name="Énfasis1" xfId="18"/>
+    <cellStyle builtinId="33" customBuiltin="1" name="Énfasis2" xfId="22"/>
+    <cellStyle builtinId="37" customBuiltin="1" name="Énfasis3" xfId="26"/>
+    <cellStyle builtinId="41" customBuiltin="1" name="Énfasis4" xfId="30"/>
+    <cellStyle builtinId="45" customBuiltin="1" name="Énfasis5" xfId="34"/>
+    <cellStyle builtinId="49" customBuiltin="1" name="Énfasis6" xfId="38"/>
+    <cellStyle builtinId="20" customBuiltin="1" name="Entrada" xfId="9"/>
+    <cellStyle builtinId="8" name="Hipervínculo" xfId="42"/>
+    <cellStyle builtinId="27" customBuiltin="1" name="Incorrecto" xfId="7"/>
+    <cellStyle builtinId="28" customBuiltin="1" name="Neutral" xfId="8"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="10" customBuiltin="1" name="Notas" xfId="15"/>
+    <cellStyle builtinId="21" customBuiltin="1" name="Salida" xfId="10"/>
+    <cellStyle builtinId="11" customBuiltin="1" name="Texto de advertencia" xfId="14"/>
+    <cellStyle builtinId="53" customBuiltin="1" name="Texto explicativo" xfId="16"/>
+    <cellStyle builtinId="15" customBuiltin="1" name="Título" xfId="1"/>
+    <cellStyle builtinId="17" customBuiltin="1" name="Título 2" xfId="3"/>
+    <cellStyle builtinId="18" customBuiltin="1" name="Título 3" xfId="4"/>
+    <cellStyle builtinId="25" customBuiltin="1" name="Total" xfId="17"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -737,10 +755,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -775,7 +793,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -827,7 +845,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -938,21 +956,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -969,7 +987,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1021,30 +1039,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="29.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="17.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="21.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="25.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="16.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="29.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="27.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1055,38 +1074,44 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>7</v>
+        <v>45</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0019CDEF-97B4-4499-A41D-540860F326F8}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0019CDEF-97B4-4499-A41D-540860F326F8}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
@@ -1094,59 +1119,176 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCBC2C18-1D40-46D1-9A86-345E56C1F6DE}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="26.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.7109375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C2" t="s">
-        <v>28</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C34B365-6246-4C0E-B4B1-4B12861E548E}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="30.28515625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58EF1752-CF33-450D-BCD7-878A30A4887B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58EF1752-CF33-450D-BCD7-878A30A4887B}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21" style="2" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="21" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="21.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="19.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="21.0" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" style="2" width="18.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="2" width="17.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="2" width="15.28515625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D484ABA6-0855-40CC-A318-BE4F264476CB}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" style="2" width="28.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="47.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="20.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="24.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="26.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="27.7109375" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -1155,61 +1297,61 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>25</v>
+      <c r="F2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D484ABA6-0855-40CC-A318-BE4F264476CB}">
-  <dimension ref="A1:E2"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{839145ED-37FD-4D66-990C-E36B19483E3A}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="47.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="20" style="2" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="26.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="21.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="23.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="22.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="16.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="19.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -1218,106 +1360,46 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>7</v>
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{839145ED-37FD-4D66-990C-E36B19483E3A}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="21.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="2"/>
-    <col min="5" max="5" width="19" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{961B6476-8C92-43E9-8F44-486E74A52A12}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{961B6476-8C92-43E9-8F44-486E74A52A12}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="38.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="33.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="27.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="24.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="38.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="23.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1325,44 +1407,44 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="2" customFormat="1">
+    </row>
+    <row customFormat="1" r="2" s="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319B4778-E3E9-408F-B070-D26A07EB60CD}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319B4778-E3E9-408F-B070-D26A07EB60CD}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
@@ -1370,45 +1452,45 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" customWidth="1"/>
-    <col min="2" max="2" width="30.5703125" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{85D3792F-65EC-42B7-BBDD-5FF3EC758C58}"/>
+    <hyperlink r:id="rId1" ref="B2" xr:uid="{85D3792F-65EC-42B7-BBDD-5FF3EC758C58}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId2" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ADDCCCF-6AB2-46AA-A7AA-8F4CA3727986}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ADDCCCF-6AB2-46AA-A7AA-8F4CA3727986}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -1416,11 +1498,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="20.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="24.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="21.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1428,39 +1510,39 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>18</v>
       </c>
       <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FB252CC-3182-4674-A162-127E69CDAA21}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FB252CC-3182-4674-A162-127E69CDAA21}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
@@ -1468,50 +1550,50 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="49.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="49.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://noprd-e2e-toms.temu.com.uy:7002/common/uobject.jsp?object=9157101132513589622" xr:uid="{09E1CD66-1B3B-4C3E-A809-9FBB24CB8F19}"/>
+    <hyperlink display="https://noprd-e2e-toms.temu.com.uy:7002/common/uobject.jsp?object=9157101132513589622" r:id="rId1" ref="B2" xr:uid="{09E1CD66-1B3B-4C3E-A809-9FBB24CB8F19}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId2" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FCFAA35-B389-4AC3-B2A7-BC50E5D70A93}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FCFAA35-B389-4AC3-B2A7-BC50E5D70A93}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="27" style="2" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="27.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1519,25 +1601,25 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commiteo a Pedido de una de las Iriannyses
</commit_message>
<xml_diff>
--- a/MyFirstTest/registers.xlsx
+++ b/MyFirstTest/registers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20344"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ipupo\Documents\GitHub\Automatizaci-nTFNU\MyFirstTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seba-OS\Documents\GitHub\Automatizaci-nTFNU\MyFirstTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{8CB5995E-E8E4-4ADD-869D-6A6EA7EBB9ED}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36"/>
+  <xr:revisionPtr documentId="13_ncr:1_{4E0CC4A5-9EF0-4BAC-BBAB-ECC2CF9D6FB2}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44"/>
   <bookViews>
-    <workbookView activeTab="3" windowHeight="7650" windowWidth="14790" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="0"/>
+    <workbookView windowHeight="12576" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
   </bookViews>
   <sheets>
     <sheet name="POTENTIAL-RESCLIENTS" r:id="rId1" sheetId="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="46">
   <si>
     <t>UAT</t>
   </si>
@@ -48,9 +48,6 @@
     <t>ADDRESS</t>
   </si>
   <si>
-    <t>Gonzalez</t>
-  </si>
-  <si>
     <t>18 de Julio</t>
   </si>
   <si>
@@ -99,15 +96,9 @@
     <t>PLC239</t>
   </si>
   <si>
-    <t>NativoAuto2Emp</t>
-  </si>
-  <si>
     <t>210712640045</t>
   </si>
   <si>
-    <t>9157161534413578912</t>
-  </si>
-  <si>
     <t>PLC281</t>
   </si>
   <si>
@@ -174,10 +165,10 @@
     <t>9155890523813779409&amp;tab=_All+Tasks</t>
   </si>
   <si>
-    <t>22222222</t>
-  </si>
-  <si>
-    <t/>
+    <t>15151lk</t>
+  </si>
+  <si>
+    <t>9157360241913802101</t>
   </si>
 </sst>
 </file>
@@ -1049,18 +1040,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="17.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="21.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="25.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="16.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="2" width="29.42578125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" style="2" width="17.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="21.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="25.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="16.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="29.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="27.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1074,10 +1065,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1085,22 +1076,22 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1117,33 +1108,33 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="21.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="23.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1159,11 +1150,11 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="26.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="20.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="26.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1171,10 +1162,10 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1190,18 +1181,18 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="30.28515625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="21.44140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="30.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1218,14 +1209,14 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" customWidth="true" style="2" width="21.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="19.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="19.6640625" collapsed="true"/>
     <col min="3" max="3" customWidth="true" style="2" width="21.0" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" style="2" width="18.85546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="2" width="17.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="2" width="15.28515625" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" style="2" width="18.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="2" width="17.44140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="2" width="15.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1242,7 +1233,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1250,16 +1241,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1276,19 +1267,19 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="28.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="47.7109375" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" style="2" width="28.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="47.6640625" collapsed="true"/>
     <col min="3" max="3" customWidth="true" style="2" width="20.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="24.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="2" width="26.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="27.7109375" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" style="2" width="24.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="26.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="27.6640625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -1297,10 +1288,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>4</v>
@@ -1308,22 +1299,22 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1336,22 +1327,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{839145ED-37FD-4D66-990C-E36B19483E3A}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="21.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="23.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="22.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="16.28515625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" style="2" width="21.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="23.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="22.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="16.33203125" collapsed="true"/>
     <col min="5" max="5" customWidth="true" style="2" width="19.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -1360,24 +1351,24 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1393,13 +1384,13 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="33.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="27.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="24.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="38.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="2" width="23.28515625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" style="2" width="33.44140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="27.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="24.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="38.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="23.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1407,33 +1398,33 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row customFormat="1" r="2" s="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1450,33 +1441,33 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="30.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="26.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="30.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1496,13 +1487,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="20.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="23.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="24.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="21.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="20.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="24.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="21.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1510,28 +1501,28 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>17</v>
       </c>
       <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1548,27 +1539,27 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="49.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.5703125" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="19.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="49.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="7"/>
     </row>
@@ -1589,11 +1580,11 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
     <col min="2" max="2" customWidth="true" style="2" width="27.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1601,21 +1592,21 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
         <v>32</v>
-      </c>
-      <c r="C2" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed - Condicion Alta PosP
</commit_message>
<xml_diff>
--- a/MyFirstTest/registers.xlsx
+++ b/MyFirstTest/registers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20344"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ipupo\Documents\GitHub\Automatizaci-nTFNU\MyFirstTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seba-OS\Documents\GitHub\Automatizaci-nTFNU\MyFirstTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C95D02-7959-4BDB-A359-1B40304EB016}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B167BD-CA32-4B8D-8338-566F8F64C7B5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="POTENTIAL-RESCLIENTS" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="47">
   <si>
     <t>UAT</t>
   </si>
@@ -108,9 +108,6 @@
     <t>NativoAuto3Emp</t>
   </si>
   <si>
-    <t>Pupo</t>
-  </si>
-  <si>
     <t>https://noprd-uat-toms.temu.com.uy:7002/common/uobject.jsp?object=9157298777113287522</t>
   </si>
   <si>
@@ -162,13 +159,19 @@
     <t>PLTTEF</t>
   </si>
   <si>
-    <t>e2e</t>
-  </si>
-  <si>
-    <t>667788554433</t>
-  </si>
-  <si>
     <t>9157366908913851340</t>
+  </si>
+  <si>
+    <t>Puper</t>
+  </si>
+  <si>
+    <t>Puper2</t>
+  </si>
+  <si>
+    <t>66778855443a</t>
+  </si>
+  <si>
+    <t>9157367657313661231</t>
   </si>
 </sst>
 </file>
@@ -1040,17 +1043,17 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="29.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="27.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="17.33203125" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.44140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.44140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="29.44140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.44140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1064,10 +1067,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1075,19 +1078,19 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>5</v>
@@ -1107,11 +1110,11 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="21.5546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1127,10 +1130,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
         <v>31</v>
-      </c>
-      <c r="B2" t="s">
-        <v>32</v>
       </c>
       <c r="C2" t="s">
         <v>23</v>
@@ -1149,11 +1152,11 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.88671875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1164,7 +1167,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1180,18 +1183,18 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="21.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1205,17 +1208,17 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="21" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.6640625" style="2" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="21" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="18.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="18.88671875" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.44140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.33203125" style="2" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1243,7 +1246,7 @@
         <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>5</v>
@@ -1266,14 +1269,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="47.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="28.6640625" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="47.6640625" style="2" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="20" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="26.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="27.7109375" customWidth="1"/>
+    <col min="4" max="4" width="24.88671875" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="26.33203125" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1287,10 +1290,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>4</v>
@@ -1298,19 +1301,19 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
@@ -1330,12 +1333,12 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="21.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="21.109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.44140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.33203125" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.33203125" style="2" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="19" style="2" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -1355,13 +1358,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>21</v>
@@ -1377,19 +1380,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{961B6476-8C92-43E9-8F44-486E74A52A12}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="33.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="38.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="33.44140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.44140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.33203125" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="38.6640625" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.33203125" style="2" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1411,19 +1414,36 @@
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1">
       <c r="A2" s="2" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>34</v>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1440,11 +1460,11 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="26.33203125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.5546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1463,7 +1483,7 @@
         <v>22</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -1486,13 +1506,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="21.109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.33203125" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.5546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1515,13 +1535,13 @@
         <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>29</v>
-      </c>
-      <c r="D2" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1538,11 +1558,11 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="49.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="19.88671875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="49.44140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1579,11 +1599,11 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="27" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1602,10 +1622,10 @@
         <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modifiaciones xpath,Arreglos en la interfaz
.
</commit_message>
<xml_diff>
--- a/MyFirstTest/registers.xlsx
+++ b/MyFirstTest/registers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ipupo\Documents\GitHub\Automatizaci-nTFNU\MyFirstTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58DB22D9-D215-455C-9AA6-4E42DDF04FF9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34133B13-D783-4F59-9A99-C1533ED30F72}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="POTENTIAL-RESCLIENTS" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="47">
   <si>
     <t>UAT</t>
   </si>
@@ -129,12 +129,6 @@
     <t>https://noprd-uat-toms.temu.com.uy:7002/common/uobject.jsp?object=9157332706713843846</t>
   </si>
   <si>
-    <t>89598071103029413716</t>
-  </si>
-  <si>
-    <t>93655923</t>
-  </si>
-  <si>
     <t>LINE</t>
   </si>
   <si>
@@ -156,9 +150,6 @@
     <t>9155890523813779409&amp;tab=_All+Tasks</t>
   </si>
   <si>
-    <t>PLTTEF</t>
-  </si>
-  <si>
     <t>Puper</t>
   </si>
   <si>
@@ -174,13 +165,13 @@
     <t>9157368300713551654</t>
   </si>
   <si>
-    <t>94749750</t>
-  </si>
-  <si>
-    <t>89598076101039725801</t>
-  </si>
-  <si>
-    <t>9157359892213715755</t>
+    <t>PLC</t>
+  </si>
+  <si>
+    <t>94754900</t>
+  </si>
+  <si>
+    <t>89598076101039725728</t>
   </si>
 </sst>
 </file>
@@ -1051,7 +1042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -1076,10 +1067,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1087,19 +1078,19 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>5</v>
@@ -1176,7 +1167,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1200,10 +1191,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1255,7 +1246,7 @@
         <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>5</v>
@@ -1299,10 +1290,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>4</v>
@@ -1310,19 +1301,19 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
@@ -1367,13 +1358,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>21</v>
@@ -1389,10 +1380,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{961B6476-8C92-43E9-8F44-486E74A52A12}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1423,37 +1414,32 @@
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1">
       <c r="A2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="E2" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>33</v>
-      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="D4" s="4"/>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="D5" s="4"/>
+      <c r="E5" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Cambios PLR y PP
</commit_message>
<xml_diff>
--- a/MyFirstTest/registers.xlsx
+++ b/MyFirstTest/registers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seba-OS\Documents\GitHub\Automatizaci-nTFNU\MyFirstTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B966A67-4E43-4CAC-8367-9EF72DC153AB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38554CD3-7AE5-483C-A30C-8D4F9C5775E9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="1188" windowWidth="17280" windowHeight="8964" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3756" yWindow="1716" windowWidth="17280" windowHeight="8964" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="POTENTIAL-RESCLIENTS" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="55">
   <si>
     <t>ENVIROMENT</t>
   </si>
@@ -84,9 +84,6 @@
     <t>LINK  SO</t>
   </si>
   <si>
-    <t>Procesamiento</t>
-  </si>
-  <si>
     <t>PLC239</t>
   </si>
   <si>
@@ -126,9 +123,6 @@
     <t>Pupo</t>
   </si>
   <si>
-    <t>4455332211</t>
-  </si>
-  <si>
     <t>NativoAuto5Emp</t>
   </si>
   <si>
@@ -141,9 +135,6 @@
     <t>9157387244013333976</t>
   </si>
   <si>
-    <t>PLR</t>
-  </si>
-  <si>
     <t>PLR238</t>
   </si>
   <si>
@@ -153,44 +144,65 @@
     <t>PLR295</t>
   </si>
   <si>
-    <t>NativoAutomation 50</t>
-  </si>
-  <si>
-    <t>NativoAutomation 51</t>
-  </si>
-  <si>
-    <t>NativoAutomation 52</t>
-  </si>
-  <si>
-    <t>44553s2211</t>
-  </si>
-  <si>
-    <t>4455332x11</t>
+    <t>89598076101039941937</t>
+  </si>
+  <si>
+    <t>89598076101039941911</t>
+  </si>
+  <si>
+    <t>9155890523813779409&amp;tab=_All+Tasks</t>
+  </si>
+  <si>
+    <t>plm2</t>
+  </si>
+  <si>
+    <t>PLTTEJ</t>
+  </si>
+  <si>
+    <t>94898012</t>
+  </si>
+  <si>
+    <t>NativoAutomation 10</t>
+  </si>
+  <si>
+    <t>NativoAutomation 11</t>
+  </si>
+  <si>
+    <t>NativoAutomation 12</t>
+  </si>
+  <si>
+    <t>44553g2211</t>
+  </si>
+  <si>
+    <t>44233s2211</t>
+  </si>
+  <si>
+    <t>44az332x11</t>
+  </si>
+  <si>
+    <t>https://noprd-e2e-toms.temu.com.uy:7002/common/uobject.jsp?object=9157480896613976599</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>plm</t>
   </si>
   <si>
-    <t>89598076101039941937</t>
-  </si>
-  <si>
-    <t>89598076101039941911</t>
-  </si>
-  <si>
-    <t>9157472159313038013</t>
-  </si>
-  <si>
-    <t>9157472435413052443</t>
-  </si>
-  <si>
-    <t>https://noprd-plm-toms.temu.com.uy:7002/common/uobject.jsp?object=9157472626813062459</t>
+    <t>PLR300</t>
+  </si>
+  <si>
+    <t>PLR314</t>
+  </si>
+  <si>
+    <t>9157481352813505538</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -340,6 +352,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1079,10 +1097,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -1090,19 +1108,19 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>4</v>
@@ -1110,45 +1128,46 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="21" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -1182,13 +1201,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1219,7 +1238,7 @@
         <v>7</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1243,10 +1262,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1259,8 +1278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58EF1752-CF33-450D-BCD7-878A30A4887B}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1292,19 +1311,19 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1342,10 +1361,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>3</v>
@@ -1353,19 +1372,19 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
         <v>4</v>
@@ -1410,19 +1429,19 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
         <v>32</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1434,8 +1453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{961B6476-8C92-43E9-8F44-486E74A52A12}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1466,16 +1485,16 @@
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1">
       <c r="A2" s="2" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="E2" s="4">
         <v>94801921</v>
@@ -1483,19 +1502,19 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" s="4">
-        <v>94898012</v>
+        <v>38</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1516,8 +1535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319B4778-E3E9-408F-B070-D26A07EB60CD}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1540,13 +1559,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
         <v>50</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1592,16 +1611,16 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
         <v>35</v>
-      </c>
-      <c r="C2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1638,7 +1657,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="7"/>
     </row>
@@ -1679,13 +1698,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test ChangUSIM - Terminado
</commit_message>
<xml_diff>
--- a/MyFirstTest/registers.xlsx
+++ b/MyFirstTest/registers.xlsx
@@ -1,38 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20344"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ipupo\Documents\GitHub\Automatizaci-nTFNU\MyFirstTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seba-OS\Documents\GitHub\Automatizaci-nTFNU\MyFirstTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{39D3AFE7-0F2A-42EC-9167-2E2067A10F69}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD7FF59-77C9-4791-A57D-26FF05A4DA40}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="6" firstSheet="3" windowHeight="8850" windowWidth="17280" xWindow="4080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="2910"/>
+    <workbookView xWindow="3576" yWindow="1428" windowWidth="17496" windowHeight="10212" firstSheet="11" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="POTENTIAL-RESCLIENTS" r:id="rId1" sheetId="1"/>
-    <sheet name="POTENTIAL-ENTCLIENTS" r:id="rId2" sheetId="3"/>
-    <sheet name="REAL-RESCLIENTS" r:id="rId3" sheetId="2"/>
-    <sheet name="REAL-ENTCLIENTS" r:id="rId4" sheetId="4"/>
-    <sheet name="NEW-PLAN" r:id="rId5" sheetId="5"/>
-    <sheet name="REAL-PLAN" r:id="rId6" sheetId="6"/>
-    <sheet name="CHANGE-PLAN" r:id="rId7" sheetId="7"/>
-    <sheet name="CHANGED-PLAN" r:id="rId8" sheetId="8"/>
-    <sheet name="SIM CARD LOST" r:id="rId9" sheetId="9"/>
-    <sheet name="REGISTERED SIM CARD LOST" r:id="rId10" sheetId="10"/>
-    <sheet name="RECHARGE LINE" r:id="rId11" sheetId="11"/>
-    <sheet name="REGISTERED RECHARGE" r:id="rId12" sheetId="12"/>
-    <sheet name="CHANGE USIM" r:id="rId13" sheetId="13"/>
+    <sheet name="POTENTIAL-RESCLIENTS" sheetId="1" r:id="rId1"/>
+    <sheet name="POTENTIAL-ENTCLIENTS" sheetId="3" r:id="rId2"/>
+    <sheet name="REAL-RESCLIENTS" sheetId="2" r:id="rId3"/>
+    <sheet name="REAL-ENTCLIENTS" sheetId="4" r:id="rId4"/>
+    <sheet name="NEW-PLAN" sheetId="5" r:id="rId5"/>
+    <sheet name="REAL-PLAN" sheetId="6" r:id="rId6"/>
+    <sheet name="CHANGE-PLAN" sheetId="7" r:id="rId7"/>
+    <sheet name="CHANGED-PLAN" sheetId="8" r:id="rId8"/>
+    <sheet name="SIM CARD LOST" sheetId="9" r:id="rId9"/>
+    <sheet name="REGISTERED SIM CARD LOST" sheetId="10" r:id="rId10"/>
+    <sheet name="RECHARGE LINE" sheetId="11" r:id="rId11"/>
+    <sheet name="REGISTERED RECHARGE" sheetId="12" r:id="rId12"/>
+    <sheet name="CHANGE USIM" sheetId="13" r:id="rId13"/>
+    <sheet name="REGISTERED CHANGE USIM" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="95">
   <si>
     <t>ENVIROMENT</t>
   </si>
@@ -262,9 +263,6 @@
     <t>test</t>
   </si>
   <si>
-    <t>9147446287413870180</t>
-  </si>
-  <si>
     <t>9157635899413877747</t>
   </si>
   <si>
@@ -302,13 +300,30 @@
   </si>
   <si>
     <t>Procesamiento</t>
+  </si>
+  <si>
+    <t>NativoAuto 30</t>
+  </si>
+  <si>
+    <t>210722630077</t>
+  </si>
+  <si>
+    <t>ENVIRONMENT</t>
+  </si>
+  <si>
+    <t>89598071102044554686</t>
+  </si>
+  <si>
+    <t>9146113550113960921</t>
+  </si>
+  <si>
+    <t>PLGME4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="22">
     <font>
       <sz val="11"/>
@@ -768,108 +783,108 @@
     </border>
   </borders>
   <cellStyleXfs count="43">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="0" fontId="4" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="5" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="2" fontId="6" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="7" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="5" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="6" fontId="10" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="6" fontId="11" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="6" fillId="0" fontId="12" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="7" fontId="13" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="8" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="15" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="0" fontId="16" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="17" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="17" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="17" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="19" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="17" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="25" fontId="17" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="26" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="27" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="17" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="30" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="20" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="16" numFmtId="49" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="19" numFmtId="49" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="18" numFmtId="49" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="42"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="20" numFmtId="49" xfId="42"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="42" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle builtinId="30" customBuiltin="1" name="20% - Énfasis1" xfId="19"/>
-    <cellStyle builtinId="34" customBuiltin="1" name="20% - Énfasis2" xfId="23"/>
-    <cellStyle builtinId="38" customBuiltin="1" name="20% - Énfasis3" xfId="27"/>
-    <cellStyle builtinId="42" customBuiltin="1" name="20% - Énfasis4" xfId="31"/>
-    <cellStyle builtinId="46" customBuiltin="1" name="20% - Énfasis5" xfId="35"/>
-    <cellStyle builtinId="50" customBuiltin="1" name="20% - Énfasis6" xfId="39"/>
-    <cellStyle builtinId="31" customBuiltin="1" name="40% - Énfasis1" xfId="20"/>
-    <cellStyle builtinId="35" customBuiltin="1" name="40% - Énfasis2" xfId="24"/>
-    <cellStyle builtinId="39" customBuiltin="1" name="40% - Énfasis3" xfId="28"/>
-    <cellStyle builtinId="43" customBuiltin="1" name="40% - Énfasis4" xfId="32"/>
-    <cellStyle builtinId="47" customBuiltin="1" name="40% - Énfasis5" xfId="36"/>
-    <cellStyle builtinId="51" customBuiltin="1" name="40% - Énfasis6" xfId="40"/>
-    <cellStyle builtinId="32" customBuiltin="1" name="60% - Énfasis1" xfId="21"/>
-    <cellStyle builtinId="36" customBuiltin="1" name="60% - Énfasis2" xfId="25"/>
-    <cellStyle builtinId="40" customBuiltin="1" name="60% - Énfasis3" xfId="29"/>
-    <cellStyle builtinId="44" customBuiltin="1" name="60% - Énfasis4" xfId="33"/>
-    <cellStyle builtinId="48" customBuiltin="1" name="60% - Énfasis5" xfId="37"/>
-    <cellStyle builtinId="52" customBuiltin="1" name="60% - Énfasis6" xfId="41"/>
-    <cellStyle builtinId="26" customBuiltin="1" name="Bueno" xfId="6"/>
-    <cellStyle builtinId="22" customBuiltin="1" name="Cálculo" xfId="11"/>
-    <cellStyle builtinId="23" customBuiltin="1" name="Celda de comprobación" xfId="13"/>
-    <cellStyle builtinId="24" customBuiltin="1" name="Celda vinculada" xfId="12"/>
-    <cellStyle builtinId="16" customBuiltin="1" name="Encabezado 1" xfId="2"/>
-    <cellStyle builtinId="19" customBuiltin="1" name="Encabezado 4" xfId="5"/>
-    <cellStyle builtinId="29" customBuiltin="1" name="Énfasis1" xfId="18"/>
-    <cellStyle builtinId="33" customBuiltin="1" name="Énfasis2" xfId="22"/>
-    <cellStyle builtinId="37" customBuiltin="1" name="Énfasis3" xfId="26"/>
-    <cellStyle builtinId="41" customBuiltin="1" name="Énfasis4" xfId="30"/>
-    <cellStyle builtinId="45" customBuiltin="1" name="Énfasis5" xfId="34"/>
-    <cellStyle builtinId="49" customBuiltin="1" name="Énfasis6" xfId="38"/>
-    <cellStyle builtinId="20" customBuiltin="1" name="Entrada" xfId="9"/>
-    <cellStyle builtinId="8" name="Hipervínculo" xfId="42"/>
-    <cellStyle builtinId="27" customBuiltin="1" name="Incorrecto" xfId="7"/>
-    <cellStyle builtinId="28" customBuiltin="1" name="Neutral" xfId="8"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="10" customBuiltin="1" name="Notas" xfId="15"/>
-    <cellStyle builtinId="21" customBuiltin="1" name="Salida" xfId="10"/>
-    <cellStyle builtinId="11" customBuiltin="1" name="Texto de advertencia" xfId="14"/>
-    <cellStyle builtinId="53" customBuiltin="1" name="Texto explicativo" xfId="16"/>
-    <cellStyle builtinId="15" customBuiltin="1" name="Título" xfId="1"/>
-    <cellStyle builtinId="17" customBuiltin="1" name="Título 2" xfId="3"/>
-    <cellStyle builtinId="18" customBuiltin="1" name="Título 3" xfId="4"/>
-    <cellStyle builtinId="25" customBuiltin="1" name="Total" xfId="17"/>
+    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Hipervínculo" xfId="42" builtinId="8"/>
+    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -886,10 +901,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -924,7 +939,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -976,7 +991,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1087,21 +1102,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1118,7 +1133,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1170,28 +1185,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="17.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="29.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="25.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="16.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="2" width="29.42578125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="1" max="1" width="17.33203125" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="29" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.44140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="29.44140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.44140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1276,24 +1291,24 @@
     </row>
   </sheetData>
   <phoneticPr fontId="21" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0019CDEF-97B4-4499-A41D-540860F326F8}">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0019CDEF-97B4-4499-A41D-540860F326F8}">
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="1" max="1" width="21.5546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1334,25 +1349,25 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCBC2C18-1D40-46D1-9A86-345E56C1F6DE}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCBC2C18-1D40-46D1-9A86-345E56C1F6DE}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="20.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="26.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="12.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="2" width="18.85546875" collapsed="true"/>
+    <col min="1" max="1" width="20.33203125" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.88671875" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.6640625" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.88671875" style="2" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1390,24 +1405,24 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C34B365-6246-4C0E-B4B1-4B12861E548E}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C34B365-6246-4C0E-B4B1-4B12861E548E}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="21.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="30.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="1" max="1" width="21.44140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.33203125" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1428,25 +1443,25 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A21E8B31-6592-4FF3-AF42-DDB11A8C0DFD}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A21E8B31-6592-4FF3-AF42-DDB11A8C0DFD}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="16.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="19.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="16.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="29.7109375" collapsed="true"/>
+    <col min="1" max="1" width="16" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.88671875" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.33203125" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.6640625" style="2" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1465,40 +1480,74 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>75</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C943F5D7-B7D5-4D4D-9987-55F3DD073C46}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="14.109375" customWidth="1"/>
+    <col min="2" max="2" width="20.21875" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58EF1752-CF33-450D-BCD7-878A30A4887B}">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58EF1752-CF33-450D-BCD7-878A30A4887B}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="21.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="19.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="21.0" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" style="2" width="18.85546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="2" width="17.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="2" width="15.28515625" collapsed="true"/>
+    <col min="1" max="1" width="21" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.6640625" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="18.88671875" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.44140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.33203125" style="2" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1520,10 +1569,10 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>68</v>
@@ -1532,48 +1581,34 @@
         <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="D3" s="3"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D484ABA6-0855-40CC-A318-BE4F264476CB}">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D484ABA6-0855-40CC-A318-BE4F264476CB}">
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="28.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="47.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="20.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="24.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="2" width="26.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="27.7109375" collapsed="true"/>
+    <col min="1" max="1" width="28.6640625" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="47.6640625" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.88671875" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="26.33203125" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1618,7 +1653,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
         <v>29</v>
@@ -1638,7 +1673,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
         <v>29</v>
@@ -1657,26 +1692,26 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{839145ED-37FD-4D66-990C-E36B19483E3A}">
-  <dimension ref="A1:F8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{839145ED-37FD-4D66-990C-E36B19483E3A}">
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="36.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="23.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="22.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="16.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="2" width="19.0" collapsed="true"/>
+    <col min="1" max="1" width="36" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.44140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.33203125" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.33203125" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19" style="2" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1754,7 +1789,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" t="s">
         <v>66</v>
@@ -1768,10 +1803,10 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C8" t="s">
         <v>68</v>
@@ -1781,25 +1816,25 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{961B6476-8C92-43E9-8F44-486E74A52A12}">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{961B6476-8C92-43E9-8F44-486E74A52A12}">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="33.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="27.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="24.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="38.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="2" width="23.28515625" collapsed="true"/>
+    <col min="1" max="1" width="33.44140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.44140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.33203125" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="38.6640625" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.33203125" style="2" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1819,29 +1854,29 @@
         <v>10</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="2" spans="1:5">
+    <row r="2" spans="1:5" s="2" customFormat="1">
       <c r="A2" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>49</v>
@@ -1862,24 +1897,24 @@
       <c r="E5" s="5"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319B4778-E3E9-408F-B070-D26A07EB60CD}">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319B4778-E3E9-408F-B070-D26A07EB60CD}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="83.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="1" max="1" width="26.33203125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="83.6640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1909,7 +1944,7 @@
         <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4" t="s">
         <v>44</v>
@@ -1917,28 +1952,28 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2" xr:uid="{85D3792F-65EC-42B7-BBDD-5FF3EC758C58}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{85D3792F-65EC-42B7-BBDD-5FF3EC758C58}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId2" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ADDCCCF-6AB2-46AA-A7AA-8F4CA3727986}">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ADDCCCF-6AB2-46AA-A7AA-8F4CA3727986}">
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="20.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="23.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="24.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="1" max="1" width="21.109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.33203125" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.5546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1972,37 +2007,37 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" t="s">
         <v>86</v>
       </c>
-      <c r="D3" t="s">
-        <v>87</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FB252CC-3182-4674-A162-127E69CDAA21}">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FB252CC-3182-4674-A162-127E69CDAA21}">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="49.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.5703125" collapsed="true"/>
+    <col min="1" max="1" width="19.88671875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="49.44140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2033,42 +2068,42 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" t="s">
         <v>86</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>87</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>88</v>
-      </c>
-      <c r="D4" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://noprd-e2e-toms.temu.com.uy:7002/common/uobject.jsp?object=9157101132513589622" r:id="rId1" ref="B2" xr:uid="{09E1CD66-1B3B-4C3E-A809-9FBB24CB8F19}"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://noprd-e2e-toms.temu.com.uy:7002/common/uobject.jsp?object=9157101132513589622" xr:uid="{09E1CD66-1B3B-4C3E-A809-9FBB24CB8F19}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId2" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FCFAA35-B389-4AC3-B2A7-BC50E5D70A93}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FCFAA35-B389-4AC3-B2A7-BC50E5D70A93}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="27.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2094,7 +2129,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Verison 1.5 - Sobre issues registrados
</commit_message>
<xml_diff>
--- a/MyFirstTest/registers.xlsx
+++ b/MyFirstTest/registers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20344"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ipupo\Documents\GitHub\Automatizaci-nTFNU\MyFirstTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seba-OS\Documents\GitHub\Automatizaci-nTFNU\MyFirstTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{D227CAFB-0D53-45F2-B4D0-EBB28B8E7374}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44"/>
+  <xr:revisionPtr documentId="13_ncr:1_{8A10AF78-138E-4780-B9A6-C01A70EE4172}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView windowHeight="8850" windowWidth="17280" xWindow="4080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="2910"/>
+    <workbookView activeTab="4" windowHeight="12576" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
   </bookViews>
   <sheets>
     <sheet name="POTENTIAL-RESCLIENTS" r:id="rId1" sheetId="1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="42">
   <si>
     <t>ENVIROMENT</t>
   </si>
@@ -46,9 +46,6 @@
     <t>ADDRESS</t>
   </si>
   <si>
-    <t>18 de Julio</t>
-  </si>
-  <si>
     <t>RUT</t>
   </si>
   <si>
@@ -82,9 +79,6 @@
     <t>NAME NEW-PLAN</t>
   </si>
   <si>
-    <t>210712640045</t>
-  </si>
-  <si>
     <t>LINE</t>
   </si>
   <si>
@@ -94,238 +88,76 @@
     <t>NATIONAL ID</t>
   </si>
   <si>
-    <t>null</t>
+    <t>AMOUNT</t>
+  </si>
+  <si>
+    <t>PAYMENT METHOD</t>
+  </si>
+  <si>
+    <t>uat</t>
+  </si>
+  <si>
+    <t>STATUS</t>
+  </si>
+  <si>
+    <t>LINK RECHARGE</t>
+  </si>
+  <si>
+    <t>Efectivo</t>
+  </si>
+  <si>
+    <t>NEW PLAN</t>
+  </si>
+  <si>
+    <t>ENVIORNMENT</t>
+  </si>
+  <si>
+    <t>USIM</t>
+  </si>
+  <si>
+    <t>OBJECT_ID</t>
+  </si>
+  <si>
+    <t>NAME_PLAN</t>
+  </si>
+  <si>
+    <t>9147446335713669323</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>95555895</t>
+  </si>
+  <si>
+    <t>https://noprd-uat-toms.temu.com.uy:7002/ncobject.jsp?id=9158455722113189416</t>
+  </si>
+  <si>
+    <t>Completado</t>
   </si>
   <si>
     <t>e2e</t>
   </si>
   <si>
-    <t>Pupo</t>
-  </si>
-  <si>
-    <t>NativoAuto5Emp</t>
-  </si>
-  <si>
-    <t>PUPO</t>
-  </si>
-  <si>
-    <t>213975190053</t>
-  </si>
-  <si>
-    <t>9155890523813779409&amp;tab=_All+Tasks</t>
-  </si>
-  <si>
-    <t>PLTTEJ</t>
-  </si>
-  <si>
-    <t>NativoAutomation 10</t>
-  </si>
-  <si>
-    <t>NativoAutomation 12</t>
-  </si>
-  <si>
-    <t>https://noprd-e2e-toms.temu.com.uy:7002/common/uobject.jsp?object=9157480896613976599</t>
+    <t>9158454170913425458</t>
+  </si>
+  <si>
+    <t>PLC295</t>
+  </si>
+  <si>
+    <t>95058978</t>
+  </si>
+  <si>
+    <t>89598076102034956193</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>PLR314</t>
-  </si>
-  <si>
-    <t>AMOUNT</t>
-  </si>
-  <si>
-    <t>PAYMENT METHOD</t>
-  </si>
-  <si>
-    <t>uat</t>
-  </si>
-  <si>
-    <t>9157523983013741997</t>
-  </si>
-  <si>
-    <t>PLC280</t>
-  </si>
-  <si>
-    <t>https://noprd-uat-toms.temu.com.uy:7002/common/uobject.jsp?object=9157530524313362060</t>
+    <t>https://noprd-e2e-toms.temu.com.uy:7002/common/uobject.jsp?object=9158456520913426468</t>
   </si>
   <si>
     <t>Ok</t>
-  </si>
-  <si>
-    <t>STATUS</t>
-  </si>
-  <si>
-    <t>LINK RECHARGE</t>
-  </si>
-  <si>
-    <t>Efectivo</t>
-  </si>
-  <si>
-    <t>44553g22444</t>
-  </si>
-  <si>
-    <t>PLTTEF</t>
-  </si>
-  <si>
-    <t>9157539306513134841</t>
-  </si>
-  <si>
-    <t>89598076101039727088</t>
-  </si>
-  <si>
-    <t>94486197</t>
-  </si>
-  <si>
-    <t>95092548</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>NO GENERO RECARGA</t>
-  </si>
-  <si>
-    <t>9147446274213489944</t>
-  </si>
-  <si>
-    <t>PLC300</t>
-  </si>
-  <si>
-    <t>PLKI32</t>
-  </si>
-  <si>
-    <t>PLC309</t>
-  </si>
-  <si>
-    <t>https://noprd-e2e-toms.temu.com.uy:7002/common/uobject.jsp?object=9157610208713394915</t>
-  </si>
-  <si>
-    <t>En Error</t>
-  </si>
-  <si>
-    <t>NEW PLAN</t>
-  </si>
-  <si>
-    <t>210722630042</t>
-  </si>
-  <si>
-    <t>213975190010</t>
-  </si>
-  <si>
-    <t>NativoAuto 1</t>
-  </si>
-  <si>
-    <t>NativoAuto 2</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>9157610519313471812</t>
-  </si>
-  <si>
-    <t>9157610556913481043</t>
-  </si>
-  <si>
-    <t>ENVIORNMENT</t>
-  </si>
-  <si>
-    <t>USIM</t>
-  </si>
-  <si>
-    <t>OBJECT_ID</t>
-  </si>
-  <si>
-    <t>NAME_PLAN</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>9147446287413870180</t>
-  </si>
-  <si>
-    <t>9157635899413877747</t>
-  </si>
-  <si>
-    <t>9157635909813404609</t>
-  </si>
-  <si>
-    <t>9157636013013430552</t>
-  </si>
-  <si>
-    <t>preprod</t>
-  </si>
-  <si>
-    <t>NativoAuto 3</t>
-  </si>
-  <si>
-    <t>9157635937013883486</t>
-  </si>
-  <si>
-    <t>89598076102034958108</t>
-  </si>
-  <si>
-    <t>95059314</t>
-  </si>
-  <si>
-    <t>https://pretoms.temu.com.uy/common/uobject.jsp?object=9157636379613954271</t>
-  </si>
-  <si>
-    <t>PLRE1</t>
-  </si>
-  <si>
-    <t>PLC2</t>
-  </si>
-  <si>
-    <t>https://pretoms.temu.com.uy/common/uobject.jsp?object=9157636639913996805</t>
-  </si>
-  <si>
-    <t>Procesamiento</t>
-  </si>
-  <si>
-    <t>9157936148413880029</t>
-  </si>
-  <si>
-    <t>PLC28</t>
-  </si>
-  <si>
-    <t>3344rrffccss221</t>
-  </si>
-  <si>
-    <t>9158023207913892838</t>
-  </si>
-  <si>
-    <t>PLR315</t>
-  </si>
-  <si>
-    <t>https://noprd-e2e-toms.temu.com.uy:7002/common/uobject.jsp?object=9158023207913892890</t>
-  </si>
-  <si>
-    <t>9158023688213894465</t>
-  </si>
-  <si>
-    <t>NativoAutomation 13</t>
-  </si>
-  <si>
-    <t>77uuii8899wwee</t>
-  </si>
-  <si>
-    <t>9158024229713895586</t>
-  </si>
-  <si>
-    <t>77uuii8899wwek</t>
-  </si>
-  <si>
-    <t>9158024321913895741</t>
-  </si>
-  <si>
-    <t>77uuii8899wwenn</t>
   </si>
 </sst>
 </file>
@@ -836,7 +668,7 @@
     <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="20" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="16" numFmtId="49" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
@@ -845,7 +677,6 @@
     <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="18" numFmtId="49" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="42"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="20" numFmtId="49" xfId="42"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle builtinId="30" customBuiltin="1" name="20% - Énfasis1" xfId="19"/>
@@ -1204,18 +1035,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="17.28515625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" style="2" width="17.33203125" collapsed="true"/>
     <col min="2" max="2" customWidth="true" style="2" width="29.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="25.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="16.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="2" width="29.42578125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="25.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="16.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="29.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="27.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1229,34 +1060,17 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="F2" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="21" type="noConversion"/>
@@ -1267,54 +1081,28 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0019CDEF-97B4-4499-A41D-540860F326F8}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A2:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="21.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="23.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1327,16 +1115,16 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="20.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="26.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="12.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="2" width="18.85546875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" style="2" width="20.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="26.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="20.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="12.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="18.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1344,33 +1132,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>48</v>
+        <v>29</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1381,34 +1169,42 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C34B365-6246-4C0E-B4B1-4B12861E548E}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="21.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="30.28515625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" style="2" width="21.44140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="30.33203125" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="19.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" t="s">
-        <v>51</v>
+      <c r="A2"/>
+      <c r="B2"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4"/>
+      <c r="B4"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1419,46 +1215,32 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A21E8B31-6592-4FF3-AF42-DDB11A8C0DFD}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" customWidth="true" style="2" width="16.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="19.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="16.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="29.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="19.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="16.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="29.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>69</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1472,17 +1254,17 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A2" sqref="A2:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" customWidth="true" style="2" width="21.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="19.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="19.6640625" collapsed="true"/>
     <col min="3" max="3" customWidth="true" style="2" width="21.0" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" style="2" width="18.85546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="2" width="17.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="2" width="15.28515625" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" style="2" width="18.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="2" width="17.44140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="2" width="15.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1499,42 +1281,14 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>60</v>
-      </c>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>60</v>
-      </c>
+      <c r="D3" s="3"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -1544,25 +1298,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D484ABA6-0855-40CC-A318-BE4F264476CB}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="28.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="47.7109375" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" style="2" width="28.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="47.6640625" collapsed="true"/>
     <col min="3" max="3" customWidth="true" style="2" width="20.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="24.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="2" width="26.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="27.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="24.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="26.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="27.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1571,154 +1325,63 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-    </row>
     <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A4"/>
+      <c r="B4"/>
+      <c r="C4"/>
+      <c r="D4"/>
+      <c r="E4"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>88</v>
-      </c>
-      <c r="B6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>93</v>
-      </c>
-      <c r="E7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>94</v>
-      </c>
-      <c r="B8" t="s">
-        <v>92</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>96</v>
-      </c>
-      <c r="B9" t="s">
-        <v>92</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" t="s">
-        <v>97</v>
-      </c>
-      <c r="E9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" t="s">
-        <v>4</v>
-      </c>
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5"/>
+      <c r="D5"/>
+      <c r="E5"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6"/>
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="D6"/>
+      <c r="E6"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7"/>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8"/>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -1731,21 +1394,21 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A2" sqref="A2:E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" customWidth="true" style="2" width="36.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="23.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="22.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="16.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="23.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="22.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="16.33203125" collapsed="true"/>
     <col min="5" max="5" customWidth="true" style="2" width="19.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1754,95 +1417,41 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>25</v>
-      </c>
+      <c r="E2"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" t="s">
-        <v>60</v>
-      </c>
+      <c r="A4"/>
+      <c r="B4"/>
+      <c r="C4"/>
+      <c r="D4"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D5" t="s">
-        <v>60</v>
-      </c>
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5"/>
+      <c r="D5"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" t="s">
-        <v>59</v>
-      </c>
+      <c r="A6"/>
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="D6"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" t="s">
-        <v>59</v>
-      </c>
+      <c r="A7"/>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>77</v>
-      </c>
-      <c r="B8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8" t="s">
-        <v>60</v>
-      </c>
+      <c r="A8"/>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -1853,17 +1462,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{961B6476-8C92-43E9-8F44-486E74A52A12}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="33.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="27.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="24.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="38.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="2" width="23.28515625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" style="2" width="33.44140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="27.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="24.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="38.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="23.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1871,51 +1480,38 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row customFormat="1" r="2" s="2" spans="1:5">
       <c r="A2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>86</v>
+        <v>36</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>79</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>47</v>
-      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5">
       <c r="D4" s="4"/>
@@ -1933,87 +1529,65 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319B4778-E3E9-408F-B070-D26A07EB60CD}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="83.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="26.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="83.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="B2" s="7"/>
+    </row>
+    <row r="4">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C5" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2" xr:uid="{85D3792F-65EC-42B7-BBDD-5FF3EC758C58}"/>
-  </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId2" verticalDpi="300"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ADDCCCF-6AB2-46AA-A7AA-8F4CA3727986}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="20.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="23.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="24.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="21.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="20.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="24.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="21.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2021,43 +1595,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>15</v>
-      </c>
       <c r="E1" s="6"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D3" t="s">
-        <v>82</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -2067,83 +1613,55 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FB252CC-3182-4674-A162-127E69CDAA21}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A2" sqref="A2:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="49.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.5703125" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="19.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="49.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" t="s">
-        <v>84</v>
-      </c>
+      <c r="B2" s="7"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink display="https://noprd-e2e-toms.temu.com.uy:7002/common/uobject.jsp?object=9157101132513589622" r:id="rId1" ref="B2" xr:uid="{09E1CD66-1B3B-4C3E-A809-9FBB24CB8F19}"/>
-  </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId2" verticalDpi="300"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FCFAA35-B389-4AC3-B2A7-BC50E5D70A93}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
     <col min="2" max="2" customWidth="true" style="2" width="27.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2151,21 +1669,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>7</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregada Funcionalidad - Boton Refresh
</commit_message>
<xml_diff>
--- a/MyFirstTest/registers.xlsx
+++ b/MyFirstTest/registers.xlsx
@@ -1,38 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seba-OS\Documents\GitHub\Automatizaci-nTFNU\MyFirstTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{8A10AF78-138E-4780-B9A6-C01A70EE4172}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0426308-786B-4F52-A4DB-9C1D2C4128CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="4" windowHeight="12576" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
+    <workbookView xWindow="1620" yWindow="1968" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="POTENTIAL-RESCLIENTS" r:id="rId1" sheetId="1"/>
-    <sheet name="POTENTIAL-ENTCLIENTS" r:id="rId2" sheetId="3"/>
-    <sheet name="REAL-RESCLIENTS" r:id="rId3" sheetId="2"/>
-    <sheet name="REAL-ENTCLIENTS" r:id="rId4" sheetId="4"/>
-    <sheet name="NEW-PLAN" r:id="rId5" sheetId="5"/>
-    <sheet name="REAL-PLAN" r:id="rId6" sheetId="6"/>
-    <sheet name="CHANGE-PLAN" r:id="rId7" sheetId="7"/>
-    <sheet name="CHANGED-PLAN" r:id="rId8" sheetId="8"/>
-    <sheet name="SIM CARD LOST" r:id="rId9" sheetId="9"/>
-    <sheet name="REGISTERED SIM CARD LOST" r:id="rId10" sheetId="10"/>
-    <sheet name="RECHARGE LINE" r:id="rId11" sheetId="11"/>
-    <sheet name="REGISTERED RECHARGE" r:id="rId12" sheetId="12"/>
-    <sheet name="CHANGE USIM" r:id="rId13" sheetId="13"/>
+    <sheet name="POTENTIAL-RESCLIENTS" sheetId="1" r:id="rId1"/>
+    <sheet name="POTENTIAL-ENTCLIENTS" sheetId="3" r:id="rId2"/>
+    <sheet name="REAL-RESCLIENTS" sheetId="2" r:id="rId3"/>
+    <sheet name="REAL-ENTCLIENTS" sheetId="4" r:id="rId4"/>
+    <sheet name="NEW-PLAN" sheetId="5" r:id="rId5"/>
+    <sheet name="REAL-PLAN" sheetId="6" r:id="rId6"/>
+    <sheet name="CHANGE-PLAN" sheetId="7" r:id="rId7"/>
+    <sheet name="CHANGED-PLAN" sheetId="8" r:id="rId8"/>
+    <sheet name="SIM CARD LOST" sheetId="9" r:id="rId9"/>
+    <sheet name="REGISTERED SIM CARD LOST" sheetId="10" r:id="rId10"/>
+    <sheet name="RECHARGE LINE" sheetId="11" r:id="rId11"/>
+    <sheet name="REGISTERED RECHARGE" sheetId="12" r:id="rId12"/>
+    <sheet name="CHANGE USIM" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="47">
   <si>
     <t>ENVIROMENT</t>
   </si>
@@ -94,77 +94,91 @@
     <t>PAYMENT METHOD</t>
   </si>
   <si>
+    <t>STATUS</t>
+  </si>
+  <si>
+    <t>LINK RECHARGE</t>
+  </si>
+  <si>
+    <t>Efectivo</t>
+  </si>
+  <si>
+    <t>NEW PLAN</t>
+  </si>
+  <si>
+    <t>ENVIORNMENT</t>
+  </si>
+  <si>
+    <t>USIM</t>
+  </si>
+  <si>
+    <t>OBJECT_ID</t>
+  </si>
+  <si>
+    <t>NAME_PLAN</t>
+  </si>
+  <si>
+    <t>9147446335713669323</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>95555895</t>
+  </si>
+  <si>
+    <t>https://noprd-uat-toms.temu.com.uy:7002/ncobject.jsp?id=9158455722113189416</t>
+  </si>
+  <si>
+    <t>Completado</t>
+  </si>
+  <si>
+    <t>e2e</t>
+  </si>
+  <si>
+    <t>PLC295</t>
+  </si>
+  <si>
+    <t>95058978</t>
+  </si>
+  <si>
+    <t>89598076102034956193</t>
+  </si>
+  <si>
+    <t>https://noprd-e2e-toms.temu.com.uy:7002/common/uobject.jsp?object=9158456520913426468</t>
+  </si>
+  <si>
+    <t>Ok</t>
+  </si>
+  <si>
     <t>uat</t>
   </si>
   <si>
-    <t>STATUS</t>
-  </si>
-  <si>
-    <t>LINK RECHARGE</t>
-  </si>
-  <si>
-    <t>Efectivo</t>
-  </si>
-  <si>
-    <t>NEW PLAN</t>
-  </si>
-  <si>
-    <t>ENVIORNMENT</t>
-  </si>
-  <si>
-    <t>USIM</t>
-  </si>
-  <si>
-    <t>OBJECT_ID</t>
-  </si>
-  <si>
-    <t>NAME_PLAN</t>
-  </si>
-  <si>
-    <t>9147446335713669323</t>
-  </si>
-  <si>
-    <t>150</t>
-  </si>
-  <si>
-    <t>95555895</t>
-  </si>
-  <si>
-    <t>https://noprd-uat-toms.temu.com.uy:7002/ncobject.jsp?id=9158455722113189416</t>
-  </si>
-  <si>
-    <t>Completado</t>
-  </si>
-  <si>
-    <t>e2e</t>
-  </si>
-  <si>
-    <t>9158454170913425458</t>
-  </si>
-  <si>
-    <t>PLC295</t>
-  </si>
-  <si>
-    <t>95058978</t>
-  </si>
-  <si>
-    <t>89598076102034956193</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>https://noprd-e2e-toms.temu.com.uy:7002/common/uobject.jsp?object=9158456520913426468</t>
-  </si>
-  <si>
-    <t>Ok</t>
+    <t>23</t>
+  </si>
+  <si>
+    <t>PLTTEF</t>
+  </si>
+  <si>
+    <t>Nativo Test Auto</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>asd2asz</t>
+  </si>
+  <si>
+    <t>18 de julio</t>
+  </si>
+  <si>
+    <t>null</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="22">
     <font>
       <sz val="11"/>
@@ -624,107 +638,107 @@
     </border>
   </borders>
   <cellStyleXfs count="43">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="0" fontId="4" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="5" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="2" fontId="6" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="7" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="5" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="6" fontId="10" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="6" fontId="11" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="6" fillId="0" fontId="12" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="7" fontId="13" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="8" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="15" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="0" fontId="16" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="17" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="17" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="17" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="19" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="17" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="25" fontId="17" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="26" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="27" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="17" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="30" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="20" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="16" numFmtId="49" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="19" numFmtId="49" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="18" numFmtId="49" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle builtinId="30" customBuiltin="1" name="20% - Énfasis1" xfId="19"/>
-    <cellStyle builtinId="34" customBuiltin="1" name="20% - Énfasis2" xfId="23"/>
-    <cellStyle builtinId="38" customBuiltin="1" name="20% - Énfasis3" xfId="27"/>
-    <cellStyle builtinId="42" customBuiltin="1" name="20% - Énfasis4" xfId="31"/>
-    <cellStyle builtinId="46" customBuiltin="1" name="20% - Énfasis5" xfId="35"/>
-    <cellStyle builtinId="50" customBuiltin="1" name="20% - Énfasis6" xfId="39"/>
-    <cellStyle builtinId="31" customBuiltin="1" name="40% - Énfasis1" xfId="20"/>
-    <cellStyle builtinId="35" customBuiltin="1" name="40% - Énfasis2" xfId="24"/>
-    <cellStyle builtinId="39" customBuiltin="1" name="40% - Énfasis3" xfId="28"/>
-    <cellStyle builtinId="43" customBuiltin="1" name="40% - Énfasis4" xfId="32"/>
-    <cellStyle builtinId="47" customBuiltin="1" name="40% - Énfasis5" xfId="36"/>
-    <cellStyle builtinId="51" customBuiltin="1" name="40% - Énfasis6" xfId="40"/>
-    <cellStyle builtinId="32" customBuiltin="1" name="60% - Énfasis1" xfId="21"/>
-    <cellStyle builtinId="36" customBuiltin="1" name="60% - Énfasis2" xfId="25"/>
-    <cellStyle builtinId="40" customBuiltin="1" name="60% - Énfasis3" xfId="29"/>
-    <cellStyle builtinId="44" customBuiltin="1" name="60% - Énfasis4" xfId="33"/>
-    <cellStyle builtinId="48" customBuiltin="1" name="60% - Énfasis5" xfId="37"/>
-    <cellStyle builtinId="52" customBuiltin="1" name="60% - Énfasis6" xfId="41"/>
-    <cellStyle builtinId="26" customBuiltin="1" name="Bueno" xfId="6"/>
-    <cellStyle builtinId="22" customBuiltin="1" name="Cálculo" xfId="11"/>
-    <cellStyle builtinId="23" customBuiltin="1" name="Celda de comprobación" xfId="13"/>
-    <cellStyle builtinId="24" customBuiltin="1" name="Celda vinculada" xfId="12"/>
-    <cellStyle builtinId="16" customBuiltin="1" name="Encabezado 1" xfId="2"/>
-    <cellStyle builtinId="19" customBuiltin="1" name="Encabezado 4" xfId="5"/>
-    <cellStyle builtinId="29" customBuiltin="1" name="Énfasis1" xfId="18"/>
-    <cellStyle builtinId="33" customBuiltin="1" name="Énfasis2" xfId="22"/>
-    <cellStyle builtinId="37" customBuiltin="1" name="Énfasis3" xfId="26"/>
-    <cellStyle builtinId="41" customBuiltin="1" name="Énfasis4" xfId="30"/>
-    <cellStyle builtinId="45" customBuiltin="1" name="Énfasis5" xfId="34"/>
-    <cellStyle builtinId="49" customBuiltin="1" name="Énfasis6" xfId="38"/>
-    <cellStyle builtinId="20" customBuiltin="1" name="Entrada" xfId="9"/>
-    <cellStyle builtinId="8" name="Hipervínculo" xfId="42"/>
-    <cellStyle builtinId="27" customBuiltin="1" name="Incorrecto" xfId="7"/>
-    <cellStyle builtinId="28" customBuiltin="1" name="Neutral" xfId="8"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="10" customBuiltin="1" name="Notas" xfId="15"/>
-    <cellStyle builtinId="21" customBuiltin="1" name="Salida" xfId="10"/>
-    <cellStyle builtinId="11" customBuiltin="1" name="Texto de advertencia" xfId="14"/>
-    <cellStyle builtinId="53" customBuiltin="1" name="Texto explicativo" xfId="16"/>
-    <cellStyle builtinId="15" customBuiltin="1" name="Título" xfId="1"/>
-    <cellStyle builtinId="17" customBuiltin="1" name="Título 2" xfId="3"/>
-    <cellStyle builtinId="18" customBuiltin="1" name="Título 3" xfId="4"/>
-    <cellStyle builtinId="25" customBuiltin="1" name="Total" xfId="17"/>
+    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Hipervínculo" xfId="42" builtinId="8"/>
+    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -741,10 +755,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -779,7 +793,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -831,7 +845,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -942,21 +956,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -973,7 +987,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1025,28 +1039,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="17.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="29.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="25.44140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="16.109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="2" width="29.44140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="27.44140625" collapsed="true"/>
+    <col min="1" max="1" width="17.33203125" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="29" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.44140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="29.44140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.44140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1070,18 +1084,35 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="F2" s="3"/>
+      <c r="A2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="21" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0019CDEF-97B4-4499-A41D-540860F326F8}">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0019CDEF-97B4-4499-A41D-540860F326F8}">
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A2:C6"/>
@@ -1089,9 +1120,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.5546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="23.109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.5546875" collapsed="true"/>
+    <col min="1" max="1" width="21.5546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1106,25 +1137,25 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCBC2C18-1D40-46D1-9A86-345E56C1F6DE}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCBC2C18-1D40-46D1-9A86-345E56C1F6DE}">
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="20.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="26.88671875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="20.6640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="12.5546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="2" width="18.88671875" collapsed="true"/>
+    <col min="1" max="1" width="20.33203125" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.88671875" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.6640625" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.88671875" style="2" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1146,30 +1177,47 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>23</v>
+      <c r="D3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C34B365-6246-4C0E-B4B1-4B12861E548E}">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C34B365-6246-4C0E-B4B1-4B12861E548E}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G29" sqref="G29"/>
@@ -1177,17 +1225,17 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="21.44140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="30.33203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="1" max="1" width="21.44140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.33203125" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" s="6"/>
     </row>
@@ -1201,21 +1249,21 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
         <v>32</v>
       </c>
-      <c r="B5" t="s">
-        <v>33</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A21E8B31-6592-4FF3-AF42-DDB11A8C0DFD}">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A21E8B31-6592-4FF3-AF42-DDB11A8C0DFD}">
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:D2"/>
@@ -1223,35 +1271,35 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="16.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="19.88671875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="16.33203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="29.6640625" collapsed="true"/>
+    <col min="1" max="1" width="16" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.88671875" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.33203125" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.6640625" style="2" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>26</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58EF1752-CF33-450D-BCD7-878A30A4887B}">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58EF1752-CF33-450D-BCD7-878A30A4887B}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:E3"/>
@@ -1259,12 +1307,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="21.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="19.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="21.0" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" style="2" width="18.88671875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="2" width="17.44140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="2" width="15.33203125" collapsed="true"/>
+    <col min="1" max="1" width="21" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.6640625" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="18.88671875" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.44140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.33203125" style="2" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1291,14 +1339,14 @@
       <c r="D3" s="3"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D484ABA6-0855-40CC-A318-BE4F264476CB}">
-  <dimension ref="A1:G10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D484ABA6-0855-40CC-A318-BE4F264476CB}">
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:F10"/>
@@ -1306,12 +1354,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="28.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="47.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="20.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="24.88671875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="2" width="26.33203125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="27.6640625" collapsed="true"/>
+    <col min="1" max="1" width="28.6640625" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="47.6640625" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.88671875" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="26.33203125" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1384,14 +1432,14 @@
       <c r="E10"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{839145ED-37FD-4D66-990C-E36B19483E3A}">
-  <dimension ref="A1:F8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{839145ED-37FD-4D66-990C-E36B19483E3A}">
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:E8"/>
@@ -1399,11 +1447,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="36.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="23.44140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="22.33203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="16.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="2" width="19.0" collapsed="true"/>
+    <col min="1" max="1" width="36" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.44140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.33203125" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.33203125" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19" style="2" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1454,25 +1502,25 @@
       <c r="D8"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{961B6476-8C92-43E9-8F44-486E74A52A12}">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{961B6476-8C92-43E9-8F44-486E74A52A12}">
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="33.44140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="27.44140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="24.33203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="38.6640625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="2" width="23.33203125" collapsed="true"/>
+    <col min="1" max="1" width="33.44140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.44140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.33203125" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="38.6640625" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.33203125" style="2" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1492,21 +1540,21 @@
         <v>9</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="2" spans="1:5">
+    <row r="2" spans="1:5" s="2" customFormat="1">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1515,21 +1563,21 @@
     </row>
     <row r="4" spans="1:5">
       <c r="D4" s="4"/>
-      <c r="E4" s="5"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5">
       <c r="D5" s="4"/>
       <c r="E5" s="5"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319B4778-E3E9-408F-B070-D26A07EB60CD}">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319B4778-E3E9-408F-B070-D26A07EB60CD}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C5"/>
@@ -1537,9 +1585,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="83.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="24.33203125" collapsed="true"/>
+    <col min="1" max="1" width="26.33203125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="83.6640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1556,26 +1604,26 @@
     <row r="2" spans="1:3">
       <c r="B2" s="7"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ADDCCCF-6AB2-46AA-A7AA-8F4CA3727986}">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ADDCCCF-6AB2-46AA-A7AA-8F4CA3727986}">
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:D3"/>
@@ -1583,11 +1631,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="20.33203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="24.5546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="21.5546875" collapsed="true"/>
+    <col min="1" max="1" width="21.109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.33203125" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.5546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1606,14 +1654,14 @@
       <c r="E1" s="6"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FB252CC-3182-4674-A162-127E69CDAA21}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FB252CC-3182-4674-A162-127E69CDAA21}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:D4"/>
@@ -1621,9 +1669,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="49.44140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.5546875" collapsed="true"/>
+    <col min="1" max="1" width="19.88671875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="49.44140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1631,7 +1679,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>11</v>
@@ -1644,14 +1692,14 @@
       <c r="B2" s="7"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FCFAA35-B389-4AC3-B2A7-BC50E5D70A93}">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FCFAA35-B389-4AC3-B2A7-BC50E5D70A93}">
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C2"/>
@@ -1659,9 +1707,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="27.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="20.6640625" collapsed="true"/>
+    <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1676,7 +1724,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>